<commit_message>
Added 1 matplotlib pie and final tumor vol by mouse
</commit_message>
<xml_diff>
--- a/Pymaceuticals/data/study_results_complete.xlsx
+++ b/Pymaceuticals/data/study_results_complete.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KDSharp\data-science\smu-bootcamp\matplotlib-challenge\Pymaceuticals\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{9A462AE2-D7CD-44EE-83FC-3243FBC7E5FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27798A54-DADB-4815-AA4B-B0DCEC7B3A5A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1068" yWindow="-108" windowWidth="22080" windowHeight="13176"/>
+    <workbookView xWindow="1068" yWindow="-108" windowWidth="22080" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="study_results_complete" sheetId="1" r:id="rId1"/>
@@ -870,7 +870,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1744,13 +1744,13 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:P1899"/>
+  <dimension ref="A1:Q1899"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O424" sqref="O424"/>
+      <selection pane="bottomLeft" activeCell="J1" sqref="J1:K1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1760,116 +1760,116 @@
     <col min="3" max="6" width="6.109375" customWidth="1"/>
     <col min="7" max="7" width="12.21875" customWidth="1"/>
     <col min="8" max="8" width="5.77734375" customWidth="1"/>
-    <col min="10" max="10" width="5" customWidth="1"/>
-    <col min="11" max="11" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.21875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="37" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5" customWidth="1"/>
+    <col min="12" max="12" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.21875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="37" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="K1" s="1" t="s">
+    <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="L1" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="2" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="K2" s="5" t="s">
-        <v>1</v>
-      </c>
+    <row r="2" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="L2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="M2" s="5" t="s">
         <v>269</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="N2" s="5" t="s">
         <v>270</v>
       </c>
-      <c r="N2" s="5" t="s">
+      <c r="O2" s="5" t="s">
         <v>271</v>
       </c>
-      <c r="O2" s="5" t="s">
+      <c r="P2" s="5" t="s">
         <v>272</v>
       </c>
-      <c r="P2" s="5" t="s">
+      <c r="Q2" s="5" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="3" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="K3" t="s">
+    <row r="3" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="L3" t="s">
         <v>62</v>
       </c>
-      <c r="L3" s="3">
+      <c r="M3" s="3">
         <v>52.884795108595497</v>
       </c>
-      <c r="M3" s="3">
+      <c r="N3" s="3">
         <v>51.82058438</v>
       </c>
-      <c r="N3" s="3">
+      <c r="O3" s="3">
         <v>43.128684128836547</v>
       </c>
-      <c r="O3" s="3">
+      <c r="P3" s="3">
         <v>6.5672432670669769</v>
       </c>
-      <c r="P3" s="6">
+      <c r="Q3" s="6">
         <v>0.49223569380114102</v>
       </c>
     </row>
-    <row r="4" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="K4" t="s">
+    <row r="4" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="L4" t="s">
         <v>9</v>
       </c>
-      <c r="L4" s="3">
+      <c r="M4" s="3">
         <v>40.216745066710523</v>
       </c>
-      <c r="M4" s="3">
+      <c r="N4" s="3">
         <v>40.67323554</v>
       </c>
-      <c r="N4" s="3">
+      <c r="O4" s="3">
         <v>23.486703952094889</v>
       </c>
-      <c r="O4" s="3">
+      <c r="P4" s="3">
         <v>4.8463082807529787</v>
       </c>
-      <c r="P4" s="6">
+      <c r="Q4" s="6">
         <v>0.32095460650847912</v>
       </c>
     </row>
-    <row r="5" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="K5" t="s">
+    <row r="5" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="L5" t="s">
         <v>67</v>
       </c>
-      <c r="L5" s="3">
+      <c r="M5" s="3">
         <v>52.59117180960677</v>
       </c>
-      <c r="M5" s="3">
+      <c r="N5" s="3">
         <v>51.77615728</v>
       </c>
-      <c r="N5" s="3">
+      <c r="O5" s="3">
         <v>39.290177273275965</v>
       </c>
-      <c r="O5" s="3">
+      <c r="P5" s="3">
         <v>6.2681877184139889</v>
       </c>
-      <c r="P5" s="6">
+      <c r="Q5" s="6">
         <v>0.46982053275259522</v>
       </c>
     </row>
-    <row r="6" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>0</v>
       </c>
@@ -1894,26 +1894,26 @@
       <c r="H6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="K6" s="3" t="s">
+      <c r="L6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="L6" s="3">
+      <c r="M6" s="3">
         <v>40.675741140999989</v>
       </c>
-      <c r="M6" s="3">
+      <c r="N6" s="3">
         <v>41.557808879999996</v>
       </c>
-      <c r="N6" s="3">
+      <c r="O6" s="3">
         <v>24.947764120255059</v>
       </c>
-      <c r="O6" s="3">
+      <c r="P6" s="3">
         <v>4.9947736805840419</v>
       </c>
-      <c r="P6" s="3">
+      <c r="Q6" s="3">
         <v>0.32934562340083229</v>
       </c>
     </row>
-    <row r="7" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -1939,7 +1939,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -1965,7 +1965,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -1991,7 +1991,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>43</v>
       </c>
@@ -2017,7 +2017,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>43</v>
       </c>
@@ -2043,7 +2043,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>43</v>
       </c>
@@ -2069,7 +2069,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>43</v>
       </c>
@@ -2095,7 +2095,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>43</v>
       </c>
@@ -2121,7 +2121,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>43</v>
       </c>
@@ -2147,7 +2147,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>43</v>
       </c>
@@ -51132,7 +51132,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A6:H1899">
+  <autoFilter ref="A6:H1899" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <filterColumn colId="1">
       <filters>
         <filter val="Infubinol"/>
@@ -51148,10 +51148,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H64"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E25" sqref="E25"/>
     </sheetView>
@@ -52832,7 +52832,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H64"/>
+  <autoFilter ref="A1:H64" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>